<commit_message>
Added config examples for notification pacing
Added recommended configuration examples for alarm notification pacing to docs.
</commit_message>
<xml_diff>
--- a/devnotes/20151122 Reminder Timing with Quadratic Bezier Curve.xlsx
+++ b/devnotes/20151122 Reminder Timing with Quadratic Bezier Curve.xlsx
@@ -33,6 +33,7 @@
         <color rgb="FF56A8F5"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">calc_next_notification_delay_secs</t>
     </r>
@@ -43,6 +44,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(notify_every_n_secs, after_every_n_notifications, secs_since_first_notification, current_notification_index)</t>
     </r>
@@ -51,7 +53,7 @@
     <t xml:space="preserve">Slow reminders to once every:</t>
   </si>
   <si>
-    <t xml:space="preserve">minutes</t>
+    <t xml:space="preserve">seconds</t>
   </si>
   <si>
     <t xml:space="preserve">notify_every_n_secs = </t>
@@ -69,7 +71,7 @@
     <t xml:space="preserve">(Note that alarms will take</t>
   </si>
   <si>
-    <t xml:space="preserve">minutes to slow down)</t>
+    <t xml:space="preserve">Seconds to slow down)</t>
   </si>
   <si>
     <t xml:space="preserve">secs_since_first_notification = </t>
@@ -93,10 +95,10 @@
     <t xml:space="preserve">By(t)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mins Since previous alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mins since first alarm</t>
+    <t xml:space="preserve">Secs Since previous alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secs since first alarm</t>
   </si>
   <si>
     <t xml:space="preserve">QUADRATIC BEZIER CURVE POINTS (INTERNALS)</t>
@@ -196,7 +198,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,6 +235,7 @@
       <color rgb="FF56A8F5"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -240,6 +243,7 @@
       <color rgb="FFBCBEC4"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -247,12 +251,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -390,38 +388,42 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,23 +431,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,11 +459,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,7 +538,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -824,7 +826,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                       <a:solidFill>
                         <a:srgbClr val="404040"/>
                       </a:solidFill>
@@ -869,7 +871,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                       <a:solidFill>
                         <a:srgbClr val="404040"/>
                       </a:solidFill>
@@ -914,7 +916,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                       <a:solidFill>
                         <a:srgbClr val="404040"/>
                       </a:solidFill>
@@ -1037,11 +1039,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="77860594"/>
-        <c:axId val="81368260"/>
+        <c:axId val="33076223"/>
+        <c:axId val="83289969"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77860594"/>
+        <c:axId val="33076223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,12 +1119,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81368260"/>
+        <c:crossAx val="83289969"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81368260"/>
+        <c:axId val="83289969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1200,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77860594"/>
+        <c:crossAx val="33076223"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1250,7 +1252,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1262,10 +1264,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.150813993765154"/>
-          <c:y val="0.0463012813610423"/>
-          <c:w val="0.805888465535158"/>
-          <c:h val="0.697964897168084"/>
+          <c:x val="0.15082444228904"/>
+          <c:y val="0.0463255422194146"/>
+          <c:w val="0.805805736455591"/>
+          <c:h val="0.697936407664772"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1474,11 +1476,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71794143"/>
-        <c:axId val="87134766"/>
+        <c:axId val="16404062"/>
+        <c:axId val="90369206"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71794143"/>
+        <c:axId val="16404062"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,12 +1556,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87134766"/>
+        <c:crossAx val="90369206"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87134766"/>
+        <c:axId val="90369206"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,7 +1637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71794143"/>
+        <c:crossAx val="16404062"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1698,9 +1700,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
+      <xdr:colOff>48600</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1709,7 +1711,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7390800" y="261000"/>
-        <a:ext cx="5196240" cy="3296520"/>
+        <a:ext cx="5195880" cy="3296160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1728,9 +1730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>68040</xdr:colOff>
+      <xdr:colOff>67680</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1739,7 +1741,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7409880" y="3801600"/>
-        <a:ext cx="5196240" cy="3419280"/>
+        <a:ext cx="5195880" cy="3418920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1760,707 +1762,707 @@
   <dimension ref="C2:T51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="86.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="86.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="4" width="8.59"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <f aca="false">60*8</f>
         <v>480</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="2" t="n">
+      <c r="T4" s="3" t="n">
         <f aca="false">F4</f>
         <v>480</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="T5" s="2" t="n">
+      <c r="T5" s="3" t="n">
         <f aca="false">F5</f>
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <f aca="false">SUMIF(D12:D31,"&lt;=1", G12:G31)</f>
         <v>5034.66666666667</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="2" t="n">
+      <c r="T6" s="3" t="n">
         <f aca="false">H14</f>
         <v>181.333333333333</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="S7" s="7" t="s">
+      <c r="S7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="2" t="n">
+      <c r="T7" s="3" t="n">
         <f aca="false">C14</f>
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="2" t="n">
         <f aca="false">(1-$D12)*(1-$D12)*D$39+2*(1-$D12)*$D12*D$40+$D12*$D12*D$41</f>
         <v>0</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <f aca="false">(1-$D12)*(1-$D12)*E$39+2*(1-$D12)*$D12*E$40+$D12*$D12*E$41</f>
         <v>0</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="11" t="n">
         <f aca="false">IF(D12&lt;=1,F12,F$4)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="11" t="n">
         <f aca="false">G12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="8" t="n">
+      <c r="C13" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <f aca="false">1/$F$5</f>
         <v>0.0666666666666667</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="2" t="n">
         <f aca="false">(1-$D13)*(1-$D13)*D$39+2*(1-$D13)*$D13*D$40+$D13*$D13*D$41</f>
         <v>0.0666666666666667</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <f aca="false">(1-$D13)*(1-$D13)*E$39+2*(1-$D13)*$D13*E$40+$D13*$D13*E$41</f>
         <v>61.8666666666667</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="11" t="n">
         <f aca="false">IF(D13&lt;=1,F13,F$4)</f>
         <v>61.8666666666667</v>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="11" t="n">
         <f aca="false">G13+H12</f>
         <v>61.8666666666667</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="8" t="n">
+      <c r="C14" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">1/$F$5+D13</f>
         <v>0.133333333333333</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">(1-$D14)*(1-$D14)*D$39+2*(1-$D14)*$D14*D$40+$D14*$D14*D$41</f>
         <v>0.266666666666667</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">(1-$D14)*(1-$D14)*E$39+2*(1-$D14)*$D14*E$40+$D14*$D14*E$41</f>
         <v>119.466666666667</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="11" t="n">
         <f aca="false">IF(D14&lt;=1,F14,F$4)</f>
         <v>119.466666666667</v>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="11" t="n">
         <f aca="false">G14+H13</f>
         <v>181.333333333333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="8" t="n">
+      <c r="C15" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <f aca="false">1/$F$5+D14</f>
         <v>0.2</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">(1-$D15)*(1-$D15)*D$39+2*(1-$D15)*$D15*D$40+$D15*$D15*D$41</f>
         <v>0.6</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <f aca="false">(1-$D15)*(1-$D15)*E$39+2*(1-$D15)*$D15*E$40+$D15*$D15*E$41</f>
         <v>172.8</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="11" t="n">
         <f aca="false">IF(D15&lt;=1,F15,F$4)</f>
         <v>172.8</v>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="11" t="n">
         <f aca="false">G15+H14</f>
         <v>354.133333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="8" t="n">
+      <c r="C16" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">1/$F$5+D15</f>
         <v>0.266666666666667</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">(1-$D16)*(1-$D16)*D$39+2*(1-$D16)*$D16*D$40+$D16*$D16*D$41</f>
         <v>1.06666666666667</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <f aca="false">(1-$D16)*(1-$D16)*E$39+2*(1-$D16)*$D16*E$40+$D16*$D16*E$41</f>
         <v>221.866666666667</v>
       </c>
-      <c r="G16" s="10" t="n">
+      <c r="G16" s="11" t="n">
         <f aca="false">IF(D16&lt;=1,F16,F$4)</f>
         <v>221.866666666667</v>
       </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="11" t="n">
         <f aca="false">G16+H15</f>
         <v>576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="8" t="n">
+      <c r="C17" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">1/$F$5+D16</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="2" t="n">
         <f aca="false">(1-$D17)*(1-$D17)*D$39+2*(1-$D17)*$D17*D$40+$D17*$D17*D$41</f>
         <v>1.66666666666667</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
         <f aca="false">(1-$D17)*(1-$D17)*E$39+2*(1-$D17)*$D17*E$40+$D17*$D17*E$41</f>
         <v>266.666666666667</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="G17" s="11" t="n">
         <f aca="false">IF(D17&lt;=1,F17,F$4)</f>
         <v>266.666666666667</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="11" t="n">
         <f aca="false">G17+H16</f>
         <v>842.666666666667</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2" t="n">
         <f aca="false">1/$F$5+D17</f>
         <v>0.4</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="2" t="n">
         <f aca="false">(1-$D18)*(1-$D18)*D$39+2*(1-$D18)*$D18*D$40+$D18*$D18*D$41</f>
         <v>2.4</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
         <f aca="false">(1-$D18)*(1-$D18)*E$39+2*(1-$D18)*$D18*E$40+$D18*$D18*E$41</f>
         <v>307.2</v>
       </c>
-      <c r="G18" s="10" t="n">
+      <c r="G18" s="11" t="n">
         <f aca="false">IF(D18&lt;=1,F18,F$4)</f>
         <v>307.2</v>
       </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="11" t="n">
         <f aca="false">G18+H17</f>
         <v>1149.86666666667</v>
       </c>
-      <c r="S18" s="0" t="n">
+      <c r="S18" s="2" t="n">
         <f aca="false">0/15</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8" t="n">
+      <c r="C19" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="2" t="n">
         <f aca="false">1/$F$5+D18</f>
         <v>0.466666666666667</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="2" t="n">
         <f aca="false">(1-$D19)*(1-$D19)*D$39+2*(1-$D19)*$D19*D$40+$D19*$D19*D$41</f>
         <v>3.26666666666667</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
         <f aca="false">(1-$D19)*(1-$D19)*E$39+2*(1-$D19)*$D19*E$40+$D19*$D19*E$41</f>
         <v>343.466666666667</v>
       </c>
-      <c r="G19" s="10" t="n">
+      <c r="G19" s="11" t="n">
         <f aca="false">IF(D19&lt;=1,F19,F$4)</f>
         <v>343.466666666667</v>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="11" t="n">
         <f aca="false">G19+H18</f>
         <v>1493.33333333333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="8" t="n">
+      <c r="C20" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="2" t="n">
         <f aca="false">1/$F$5+D19</f>
         <v>0.533333333333333</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="2" t="n">
         <f aca="false">(1-$D20)*(1-$D20)*D$39+2*(1-$D20)*$D20*D$40+$D20*$D20*D$41</f>
         <v>4.26666666666667</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
         <f aca="false">(1-$D20)*(1-$D20)*E$39+2*(1-$D20)*$D20*E$40+$D20*$D20*E$41</f>
         <v>375.466666666667</v>
       </c>
-      <c r="G20" s="10" t="n">
+      <c r="G20" s="11" t="n">
         <f aca="false">IF(D20&lt;=1,F20,F$4)</f>
         <v>375.466666666667</v>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="11" t="n">
         <f aca="false">G20+H19</f>
         <v>1868.8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="8" t="n">
+      <c r="C21" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <f aca="false">1/$F$5+D20</f>
         <v>0.6</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="2" t="n">
         <f aca="false">(1-$D21)*(1-$D21)*D$39+2*(1-$D21)*$D21*D$40+$D21*$D21*D$41</f>
         <v>5.4</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
         <f aca="false">(1-$D21)*(1-$D21)*E$39+2*(1-$D21)*$D21*E$40+$D21*$D21*E$41</f>
         <v>403.2</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="11" t="n">
         <f aca="false">IF(D21&lt;=1,F21,F$4)</f>
         <v>403.2</v>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="11" t="n">
         <f aca="false">G21+H20</f>
         <v>2272</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="8" t="n">
+      <c r="C22" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="2" t="n">
         <f aca="false">1/$F$5+D21</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="2" t="n">
         <f aca="false">(1-$D22)*(1-$D22)*D$39+2*(1-$D22)*$D22*D$40+$D22*$D22*D$41</f>
         <v>6.66666666666667</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
         <f aca="false">(1-$D22)*(1-$D22)*E$39+2*(1-$D22)*$D22*E$40+$D22*$D22*E$41</f>
         <v>426.666666666667</v>
       </c>
-      <c r="G22" s="10" t="n">
+      <c r="G22" s="11" t="n">
         <f aca="false">IF(D22&lt;=1,F22,F$4)</f>
         <v>426.666666666667</v>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="H22" s="11" t="n">
         <f aca="false">G22+H21</f>
         <v>2698.66666666667</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="8" t="n">
+      <c r="C23" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="2" t="n">
         <f aca="false">1/$F$5+D22</f>
         <v>0.733333333333333</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="2" t="n">
         <f aca="false">(1-$D23)*(1-$D23)*D$39+2*(1-$D23)*$D23*D$40+$D23*$D23*D$41</f>
         <v>8.06666666666667</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="2" t="n">
         <f aca="false">(1-$D23)*(1-$D23)*E$39+2*(1-$D23)*$D23*E$40+$D23*$D23*E$41</f>
         <v>445.866666666667</v>
       </c>
-      <c r="G23" s="10" t="n">
+      <c r="G23" s="11" t="n">
         <f aca="false">IF(D23&lt;=1,F23,F$4)</f>
         <v>445.866666666667</v>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="11" t="n">
         <f aca="false">G23+H22</f>
         <v>3144.53333333333</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="8" t="n">
+      <c r="C24" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="2" t="n">
         <f aca="false">1/$F$5+D23</f>
         <v>0.8</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="2" t="n">
         <f aca="false">(1-$D24)*(1-$D24)*D$39+2*(1-$D24)*$D24*D$40+$D24*$D24*D$41</f>
         <v>9.6</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="2" t="n">
         <f aca="false">(1-$D24)*(1-$D24)*E$39+2*(1-$D24)*$D24*E$40+$D24*$D24*E$41</f>
         <v>460.8</v>
       </c>
-      <c r="G24" s="10" t="n">
+      <c r="G24" s="11" t="n">
         <f aca="false">IF(D24&lt;=1,F24,F$4)</f>
         <v>460.8</v>
       </c>
-      <c r="H24" s="10" t="n">
+      <c r="H24" s="11" t="n">
         <f aca="false">G24+H23</f>
         <v>3605.33333333333</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="8" t="n">
+      <c r="C25" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="2" t="n">
         <f aca="false">1/$F$5+D24</f>
         <v>0.866666666666667</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="2" t="n">
         <f aca="false">(1-$D25)*(1-$D25)*D$39+2*(1-$D25)*$D25*D$40+$D25*$D25*D$41</f>
         <v>11.2666666666667</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="2" t="n">
         <f aca="false">(1-$D25)*(1-$D25)*E$39+2*(1-$D25)*$D25*E$40+$D25*$D25*E$41</f>
         <v>471.466666666667</v>
       </c>
-      <c r="G25" s="10" t="n">
+      <c r="G25" s="11" t="n">
         <f aca="false">IF(D25&lt;=1,F25,F$4)</f>
         <v>471.466666666667</v>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="11" t="n">
         <f aca="false">G25+H24</f>
         <v>4076.8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="8" t="n">
+      <c r="C26" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="2" t="n">
         <f aca="false">1/$F$5+D25</f>
         <v>0.933333333333333</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="2" t="n">
         <f aca="false">(1-$D26)*(1-$D26)*D$39+2*(1-$D26)*$D26*D$40+$D26*$D26*D$41</f>
         <v>13.0666666666667</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="2" t="n">
         <f aca="false">(1-$D26)*(1-$D26)*E$39+2*(1-$D26)*$D26*E$40+$D26*$D26*E$41</f>
         <v>477.866666666667</v>
       </c>
-      <c r="G26" s="10" t="n">
+      <c r="G26" s="11" t="n">
         <f aca="false">IF(D26&lt;=1,F26,F$4)</f>
         <v>477.866666666667</v>
       </c>
-      <c r="H26" s="10" t="n">
+      <c r="H26" s="11" t="n">
         <f aca="false">G26+H25</f>
         <v>4554.66666666667</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="8" t="n">
+      <c r="C27" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="2" t="n">
         <f aca="false">1/$F$5+D26</f>
         <v>1</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="2" t="n">
         <f aca="false">(1-$D27)*(1-$D27)*D$39+2*(1-$D27)*$D27*D$40+$D27*$D27*D$41</f>
         <v>15</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="2" t="n">
         <f aca="false">(1-$D27)*(1-$D27)*E$39+2*(1-$D27)*$D27*E$40+$D27*$D27*E$41</f>
         <v>480</v>
       </c>
-      <c r="G27" s="10" t="n">
+      <c r="G27" s="11" t="n">
         <f aca="false">IF(D27&lt;=1,F27,F$4)</f>
         <v>480</v>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="11" t="n">
         <f aca="false">G27+H26</f>
         <v>5034.66666666667</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="8" t="n">
+      <c r="C28" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="2" t="n">
         <f aca="false">1/$F$5+D27</f>
         <v>1.06666666666667</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="2" t="n">
         <f aca="false">(1-$D28)*(1-$D28)*D$39+2*(1-$D28)*$D28*D$40+$D28*$D28*D$41</f>
         <v>17.0666666666667</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">(1-$D28)*(1-$D28)*E$39+2*(1-$D28)*$D28*E$40+$D28*$D28*E$41</f>
         <v>477.866666666667</v>
       </c>
-      <c r="G28" s="10" t="n">
+      <c r="G28" s="11" t="n">
         <f aca="false">IF(D28&lt;=1,F28,F$4)</f>
         <v>480</v>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="H28" s="11" t="n">
         <f aca="false">G28+H27</f>
         <v>5514.66666666667</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="8" t="n">
+      <c r="C29" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="2" t="n">
         <f aca="false">1/$F$5+D28</f>
         <v>1.13333333333333</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="2" t="n">
         <f aca="false">(1-$D29)*(1-$D29)*D$39+2*(1-$D29)*$D29*D$40+$D29*$D29*D$41</f>
         <v>19.2666666666667</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="2" t="n">
         <f aca="false">(1-$D29)*(1-$D29)*E$39+2*(1-$D29)*$D29*E$40+$D29*$D29*E$41</f>
         <v>471.466666666667</v>
       </c>
-      <c r="G29" s="10" t="n">
+      <c r="G29" s="11" t="n">
         <f aca="false">IF(D29&lt;=1,F29,F$4)</f>
         <v>480</v>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="H29" s="11" t="n">
         <f aca="false">G29+H28</f>
         <v>5994.66666666667</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="8" t="n">
+      <c r="C30" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="2" t="n">
         <f aca="false">1/$F$5+D29</f>
         <v>1.2</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="2" t="n">
         <f aca="false">(1-$D30)*(1-$D30)*D$39+2*(1-$D30)*$D30*D$40+$D30*$D30*D$41</f>
         <v>21.6</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="2" t="n">
         <f aca="false">(1-$D30)*(1-$D30)*E$39+2*(1-$D30)*$D30*E$40+$D30*$D30*E$41</f>
         <v>460.8</v>
       </c>
-      <c r="G30" s="10" t="n">
+      <c r="G30" s="11" t="n">
         <f aca="false">IF(D30&lt;=1,F30,F$4)</f>
         <v>480</v>
       </c>
-      <c r="H30" s="10" t="n">
+      <c r="H30" s="11" t="n">
         <f aca="false">G30+H29</f>
         <v>6474.66666666667</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="8" t="n">
+      <c r="C31" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="2" t="n">
         <f aca="false">1/$F$5+D30</f>
         <v>1.26666666666667</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="2" t="n">
         <f aca="false">(1-$D31)*(1-$D31)*D$39+2*(1-$D31)*$D31*D$40+$D31*$D31*D$41</f>
         <v>24.0666666666667</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="2" t="n">
         <f aca="false">(1-$D31)*(1-$D31)*E$39+2*(1-$D31)*$D31*E$40+$D31*$D31*E$41</f>
         <v>445.866666666667</v>
       </c>
-      <c r="G31" s="10" t="n">
+      <c r="G31" s="11" t="n">
         <f aca="false">IF(D31&lt;=1,F31,F$4)</f>
         <v>480</v>
       </c>
-      <c r="H31" s="10" t="n">
+      <c r="H31" s="11" t="n">
         <f aca="false">G31+H30</f>
         <v>6954.66666666667</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="2" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="2" t="n">
         <f aca="false">F4</f>
         <v>480</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="2" t="n">
         <f aca="false">F5</f>
         <v>15</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="2" t="n">
         <f aca="false">F4</f>
         <v>480</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="455.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>